<commit_message>
Fixed errors and added CSV decoding context parameters
</commit_message>
<xml_diff>
--- a/tests/Resources/encoded.xlsx
+++ b/tests/Resources/encoded.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\www\dev\Ang3\Component\php-excel-encoder\tests\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11520"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet_0" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet_0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="999999"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Hello</t>
   </si>
@@ -35,23 +39,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -62,31 +58,40 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -376,36 +381,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="4.570313" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="6.998291" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="8.140869" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="31.706543" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="24.708252" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="18.709717" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="11.711426" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="15.281982" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="31.706543" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="31.706543" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="25.85083" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="16.424561" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="str">
         <f>"bool"</f>
         <v>bool</v>
@@ -467,7 +468,7 @@
         <v>array.array.0</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -475,7 +476,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1.618</v>
+        <v>1.6180000000000001</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -515,17 +516,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix encode method and update tests
</commit_message>
<xml_diff>
--- a/tests/Resources/encoded.xlsx
+++ b/tests/Resources/encoded.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11520" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet_0" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
   <si>
     <t>Hello</t>
   </si>
@@ -384,8 +385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,4 +520,128 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="str">
+        <f>"bool"</f>
+        <v>bool</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f>"int"</f>
+        <v>int</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <f>"float"</f>
+        <v>float</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <f>"string"</f>
+        <v>string</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <f>"object.date"</f>
+        <v>object.date</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <f>"object.timezone_type"</f>
+        <v>object.timezone_type</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <f>"object.timezone"</f>
+        <v>object.timezone</v>
+      </c>
+      <c r="H1" s="1" t="str">
+        <f>"array.bool"</f>
+        <v>array.bool</v>
+      </c>
+      <c r="I1" s="1" t="str">
+        <f>"array.int"</f>
+        <v>array.int</v>
+      </c>
+      <c r="J1" s="1" t="str">
+        <f>"array.float"</f>
+        <v>array.float</v>
+      </c>
+      <c r="K1" s="1" t="str">
+        <f>"array.string"</f>
+        <v>array.string</v>
+      </c>
+      <c r="L1" s="1" t="str">
+        <f>"array.object.date"</f>
+        <v>array.object.date</v>
+      </c>
+      <c r="M1" s="1" t="str">
+        <f>"array.object.timezone_type"</f>
+        <v>array.object.timezone_type</v>
+      </c>
+      <c r="N1" s="1" t="str">
+        <f>"array.object.timezone"</f>
+        <v>array.object.timezone</v>
+      </c>
+      <c r="O1" s="1" t="str">
+        <f>"array.array.0"</f>
+        <v>array.array.0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.6180000000000001</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>3.14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>